<commit_message>
[Update] Enum Description feature
</commit_message>
<xml_diff>
--- a/Assets/Excels/Examples/Include Enum/Enum.xlsx
+++ b/Assets/Excels/Examples/Include Enum/Enum.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\sparta_team\Team12SoloProject\Assets\@Excels\Examples\Include Enum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\unity-excel-to-json\Assets\Excels\Examples\Include Enum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD628CD8-F418-40A4-9328-47DEF2A45D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302E6910-2B0B-4CDF-AF7E-B040689C37CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51630" yWindow="1620" windowWidth="23310" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enum" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Red</t>
   </si>
@@ -49,6 +49,38 @@
   </si>
   <si>
     <t>Colors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#My colors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Green!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blue!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#My sizes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>small~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>medium~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>large~</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -377,13 +409,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.08203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
@@ -401,16 +439,44 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>